<commit_message>
IMPROVE: remove str from Economic activity data
</commit_message>
<xml_diff>
--- a/src/economicActivityAggregate/assets/report.xlsx
+++ b/src/economicActivityAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>aggregate Economic Activities Index: has a format error on índices do volume de negócios</t>
+    <t>aggregate Economic Activities: has a format error on energia,água e san</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44828.87569972411</v>
+        <v>44829.4252286966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Intro AWS Textextract
</commit_message>
<xml_diff>
--- a/src/economicActivityAggregate/assets/report.xlsx
+++ b/src/economicActivityAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Database failed to get business-confidence-aggregate update date</t>
+    <t>Could not fetch the Economic Activities Index, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-actividades-economicas-iae</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44831.60458203166</v>
+        <v>44834.75732836167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IMPROVE: Using ML to match string
</commit_message>
<xml_diff>
--- a/src/economicActivityAggregate/assets/report.xlsx
+++ b/src/economicActivityAggregate/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not fetch the Economic Activities Index, the url is http://www.ine.gov.mz/estatisticas/estatisticas-economicas/indice-de-actividades-economicas-iae</t>
+    <t>aggregate Economic Activities Index: has a format error on aloj.rest. similares</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44835.04952747619</v>
+        <v>44835.13390795871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>